<commit_message>
Allow calculation of ratio for multiple values per variable
</commit_message>
<xml_diff>
--- a/www/template.xlsx
+++ b/www/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vuw-my.sharepoint.com/personal/fleminte_staff_vuw_ac_nz/Documents/3 a Res_HRC data/ShinyApps/PrevReport/www/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vuw-my.sharepoint.com/personal/fleminte_staff_vuw_ac_nz/Documents/3 a Res_HRC data/PrevReport/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1197" documentId="8_{63ADBA71-B2C1-4A75-A341-BB6113656299}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F64452D8-C386-4544-B4F0-A1F8C2EC51D8}"/>
+  <xr:revisionPtr revIDLastSave="1202" documentId="8_{63ADBA71-B2C1-4A75-A341-BB6113656299}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2A17F708-3BAF-4602-A633-021AA985D5E7}"/>
   <bookViews>
-    <workbookView xWindow="4035" yWindow="1530" windowWidth="21240" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="188">
   <si>
     <t>title</t>
   </si>
@@ -621,6 +621,18 @@
   </si>
   <si>
     <t>Emotional health</t>
+  </si>
+  <si>
+    <t>Culture</t>
+  </si>
+  <si>
+    <t>Samoa8</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>Somewhat or very proud of being Samoan</t>
   </si>
 </sst>
 </file>
@@ -685,7 +697,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -986,7 +1008,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,7 +1076,18 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -1063,19 +1096,22 @@
   <autoFilter ref="A1:D6" xr:uid="{685C397F-0D47-4A08-A4DB-9D594E3BED54}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A2:A4">
-    <cfRule type="expression" dxfId="2" priority="22">
+    <cfRule type="expression" dxfId="3" priority="24">
       <formula>_xlfn.ISFORMULA(A2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5">
-    <cfRule type="expression" dxfId="1" priority="6">
-      <formula>_xlfn.ISFORMULA(A5)</formula>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>_xlfn.ISFORMULA(A6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="0" priority="5">
-      <formula>_xlfn.ISFORMULA(A6)</formula>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="containsBlanks" priority="2" stopIfTrue="1">
+      <formula>LEN(TRIM(A5))=0</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1982,18 +2018,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2220,14 +2256,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABCE2DE6-17B5-4BB3-9252-EC9FC8DD82FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDBF97FC-5657-4433-9412-4B0BB8609358}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -2240,6 +2268,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="1ea9f476-e5d7-46f3-a780-376ee5ddd2ee"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABCE2DE6-17B5-4BB3-9252-EC9FC8DD82FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
update template to include required field - footnote
</commit_message>
<xml_diff>
--- a/www/template.xlsx
+++ b/www/template.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vuw-my.sharepoint.com/personal/fleminte_staff_vuw_ac_nz/Documents/3 a Res_HRC data/PrevReport/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1202" documentId="8_{63ADBA71-B2C1-4A75-A341-BB6113656299}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2A17F708-3BAF-4602-A633-021AA985D5E7}"/>
+  <xr:revisionPtr revIDLastSave="1209" documentId="8_{63ADBA71-B2C1-4A75-A341-BB6113656299}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{299C6D0D-E6F9-4C99-B2AF-37140B09DE15}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29700" yWindow="3330" windowWidth="27000" windowHeight="12495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
     <sheet name="all coded variables" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">variables!$A$1:$D$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">variables!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="190">
   <si>
     <t>title</t>
   </si>
@@ -632,7 +632,13 @@
     <t>2,3</t>
   </si>
   <si>
-    <t>Somewhat or very proud of being Samoan</t>
+    <t>footnote</t>
+  </si>
+  <si>
+    <t>Proud of being Samoan*</t>
+  </si>
+  <si>
+    <t>*Somewhat proud or very proud</t>
   </si>
 </sst>
 </file>
@@ -697,7 +703,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -705,13 +711,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1005,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,9 +1016,10 @@
     <col min="2" max="2" width="6.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="79.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="76.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1032,8 +1032,11 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1047,7 +1050,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1061,7 +1064,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1075,7 +1078,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>185</v>
       </c>
@@ -1083,20 +1086,23 @@
         <v>186</v>
       </c>
       <c r="C5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D5" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D6" xr:uid="{685C397F-0D47-4A08-A4DB-9D594E3BED54}"/>
+  <autoFilter ref="A1:E1" xr:uid="{746BB84B-2657-44F5-8B6F-4A0DE3DD78D9}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A2:A4">
-    <cfRule type="expression" dxfId="3" priority="24">
+    <cfRule type="expression" dxfId="2" priority="24">
       <formula>_xlfn.ISFORMULA(A2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2018,21 +2024,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000A87E1EF3FB9FC4880E267B98BBEEEE2" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14a1b04f31e98e89b62218351a71c0ee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1ea9f476-e5d7-46f3-a780-376ee5ddd2ee" xmlns:ns4="a5d3c314-d92b-413f-ada3-7410c346d515" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7cdfab4d19c10739c104847f1cdb6897" ns3:_="" ns4:_="">
     <xsd:import namespace="1ea9f476-e5d7-46f3-a780-376ee5ddd2ee"/>
@@ -2255,32 +2246,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDBF97FC-5657-4433-9412-4B0BB8609358}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="a5d3c314-d92b-413f-ada3-7410c346d515"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1ea9f476-e5d7-46f3-a780-376ee5ddd2ee"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABCE2DE6-17B5-4BB3-9252-EC9FC8DD82FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E72A8210-9A33-47EA-AB10-F8FAA9E7FF82}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2297,4 +2278,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABCE2DE6-17B5-4BB3-9252-EC9FC8DD82FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDBF97FC-5657-4433-9412-4B0BB8609358}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="a5d3c314-d92b-413f-ada3-7410c346d515"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1ea9f476-e5d7-46f3-a780-376ee5ddd2ee"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>